<commit_message>
neon results v1 plotted, still need to adjust axis. TV thermopros written, and not looking into plotting
</commit_message>
<xml_diff>
--- a/calc/enthalpy_nist.xlsx
+++ b/calc/enthalpy_nist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/23059859_student_uwa_edu_au/Documents/UWA/05. Year 5/Semester 1/GENG5511 MPE Engineering Research Project/Project/Research_Project/GENG5511_Thesis/calc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="11_F25DC773A252ABDACC10486B59DA58A25BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF9EAAAB-C637-4375-8E16-57885CA05FF1}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="11_F25DC773A252ABDACC10486B59DA58A25BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24E8A1CA-9068-4270-A3C8-2E7A27EE5556}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Xenon" sheetId="3" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="Krypton" sheetId="2" r:id="rId3"/>
     <sheet name="krypton sub" sheetId="6" r:id="rId4"/>
     <sheet name="krypton melt" sheetId="5" r:id="rId5"/>
-    <sheet name="Argon" sheetId="1" r:id="rId6"/>
+    <sheet name="neon" sheetId="7" r:id="rId6"/>
+    <sheet name="Argon" sheetId="1" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Argon!$B$2:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Argon!$B$2:$G$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Krypton!$B$2:$G$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Xenon!$B$2:$G$2</definedName>
   </definedNames>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="23">
   <si>
     <t>Temperature</t>
   </si>
@@ -112,6 +113,9 @@
   </si>
   <si>
     <t>Chen</t>
+  </si>
+  <si>
+    <t>shakeel</t>
   </si>
 </sst>
 </file>
@@ -190,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -198,6 +202,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2563,8 +2569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2C83BFD-78C4-474C-B0E8-78F23B66AF77}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection sqref="A1:D5"/>
+    <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2649,6 +2655,78 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06FF3630-2A1B-4140-98D8-A9C734AA6D1C}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5">
+        <v>7.55</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="5">
+        <v>1.88</v>
+      </c>
+      <c r="I2">
+        <v>5.3292287723346674E-12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5">
+        <v>8.9</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="I3">
+        <v>5.8482768654407568E-10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O32"/>
   <sheetViews>

</xml_diff>